<commit_message>
Added feature to read file from Front-End. DeActivate CORS permits
</commit_message>
<xml_diff>
--- a/lib/test.xlsx
+++ b/lib/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t xml:space="preserve">Sector 1</t>
   </si>
@@ -58,28 +58,19 @@
     <t xml:space="preserve">device_exp</t>
   </si>
   <si>
-    <t xml:space="preserve">Gabriel </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blanco Gutierréz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tutor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gblanco280205@crackthecode.la</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Windows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si</t>
+    <t xml:space="preserve">Javier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacheco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Padre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jepach@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PE</t>
   </si>
 </sst>
 </file>
@@ -90,11 +81,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -113,6 +105,13 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0000FF"/>
       <name val="Lucida Console"/>
       <family val="3"/>
       <charset val="1"/>
@@ -160,7 +159,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -174,6 +173,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -201,10 +204,10 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.11"/>
   </cols>
@@ -285,7 +288,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -295,35 +298,24 @@
       <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="3" t="n">
-        <v>70450297</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="4" t="n">
-        <v>38353</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="jepach@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>